<commit_message>
update outbound clicks column name
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Impressions</t>
   </si>
   <si>
-    <t xml:space="preserve">Outbound clicks</t>
+    <t xml:space="preserve">Unique outbound clicks</t>
   </si>
   <si>
     <t xml:space="preserve">Leads</t>
@@ -86,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -106,6 +106,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -151,12 +157,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,12 +296,12 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:S1"/>
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -328,7 +338,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">

</xml_diff>